<commit_message>
added return list to table2excel file
</commit_message>
<xml_diff>
--- a/DATA_1.xlsx
+++ b/DATA_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Tarun\Website wala Project\main\data-scrapping-python-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD6A8DFD-EFE1-4953-8B39-6B37501BB4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06984B9-3770-49A9-9091-9E587B689AA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5E63F44-FC91-493A-AD79-C89DC9E7FA45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{F5E63F44-FC91-493A-AD79-C89DC9E7FA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,77 +489,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63DD045-111D-44E1-921D-6425346AEBE4}">
-  <dimension ref="A3:N15"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="28.08984375" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -571,40 +603,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="3" t="s">
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new func added to excel.py
</commit_message>
<xml_diff>
--- a/DATA_1.xlsx
+++ b/DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Tarun\Website wala Project\main\data-scrapping-python-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06984B9-3770-49A9-9091-9E587B689AA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F277EF77-7E5C-4932-A378-D0403C7E25BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{F5E63F44-FC91-493A-AD79-C89DC9E7FA45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>INSTITUTE NAME </t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>BRANCH DETAILS</t>
   </si>
   <si>
     <t>S. No.</t>
@@ -76,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,26 +82,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF666666"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Garamond"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,18 +96,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -147,32 +124,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63DD045-111D-44E1-921D-6425346AEBE4}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -511,101 +472,48 @@
     <col min="13" max="13" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes to project, seems like final
</commit_message>
<xml_diff>
--- a/DATA_1.xlsx
+++ b/DATA_1.xlsx
@@ -8,53 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Tarun\Website wala Project\main\data-scrapping-python-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F277EF77-7E5C-4932-A378-D0403C7E25BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F8BCD0-5998-47AD-A4EB-BC66DB241BFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{F5E63F44-FC91-493A-AD79-C89DC9E7FA45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>S. No.</t>
+  </si>
+  <si>
+    <t>INSTITUTE CODE</t>
+  </si>
   <si>
     <t>INSTITUTE NAME </t>
   </si>
   <si>
+    <t>MOBILE </t>
+  </si>
+  <si>
+    <t>ALTERNATIVE MOBILE NUMBER</t>
+  </si>
+  <si>
+    <t>EMAIL-ID</t>
+  </si>
+  <si>
+    <t>WEBSITE</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
     <t>DISTRICT </t>
   </si>
   <si>
-    <t>EMAIL-ID</t>
-  </si>
-  <si>
-    <t>ALTERNATIVE MOBILE NUMBER</t>
-  </si>
-  <si>
-    <t>MOBILE </t>
-  </si>
-  <si>
-    <t>INSTITUTE CODE</t>
-  </si>
-  <si>
     <t>PINCODE </t>
-  </si>
-  <si>
-    <t>WEBSITE</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>S. No.</t>
   </si>
   <si>
     <t>BRANCH CODE</t>
@@ -82,6 +77,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <name val="Garamond"/>
       <family val="1"/>
@@ -449,62 +445,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63DD045-111D-44E1-921D-6425346AEBE4}">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.08984375" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -514,9 +512,45 @@
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>